<commit_message>
Economic calcuation has been complited
</commit_message>
<xml_diff>
--- a/экономика ятц/дз/бр/Ekonomicheskiy_raschyo_BR_remake.xlsx
+++ b/экономика ятц/дз/бр/Ekonomicheskiy_raschyo_BR_remake.xlsx
@@ -744,7 +744,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -754,8 +754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D261"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A245" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A233" sqref="A233"/>
+    <sheetView tabSelected="1" topLeftCell="A224" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A267" sqref="A267"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1580,7 +1580,7 @@
     </row>
     <row r="149" spans="1:2">
       <c r="A149" s="7">
-        <v>300</v>
+        <v>309</v>
       </c>
     </row>
     <row r="150" spans="1:2">
@@ -1597,7 +1597,7 @@
     <row r="153" spans="1:2">
       <c r="A153" s="7">
         <f>A149*B33</f>
-        <v>15000</v>
+        <v>15450</v>
       </c>
     </row>
     <row r="155" spans="1:2">
@@ -1844,7 +1844,7 @@
       </c>
       <c r="C223" s="6">
         <f>A221+A225-(A205*A149)/A49/1000</f>
-        <v>-2.2721101995565804E-3</v>
+        <v>-3.1002568118376275E-3</v>
       </c>
     </row>
     <row r="224" spans="1:3">
@@ -1869,11 +1869,11 @@
     <row r="229" spans="1:4">
       <c r="A229" s="6">
         <f>A217+C223</f>
-        <v>1.4261752565532596E-4</v>
+        <v>-6.8552908662572118E-4</v>
       </c>
       <c r="B229">
         <f>A229*1000</f>
-        <v>0.14261752565532596</v>
+        <v>-0.68552908662572121</v>
       </c>
     </row>
     <row r="231" spans="1:4">
@@ -1884,7 +1884,7 @@
     <row r="233" spans="1:4">
       <c r="A233" s="6">
         <f>1.25*(1.2*A229+4*A209+3.5*A213)</f>
-        <v>5.5663160776798865E-2</v>
+        <v>5.4420940858377287E-2</v>
       </c>
     </row>
     <row r="235" spans="1:4">
@@ -1901,15 +1901,15 @@
     <row r="237" spans="1:4">
       <c r="A237">
         <f>A57*D237*A197*B13 * 10</f>
-        <v>53673437.256090872</v>
+        <v>196990173.76780099</v>
       </c>
       <c r="B237">
         <f>A237/10000000</f>
-        <v>5.3673437256090875</v>
+        <v>19.699017376780098</v>
       </c>
       <c r="D237">
-        <f>2*B30+A73/B6</f>
-        <v>0.95363655355597343</v>
+        <f>2*B30+B18</f>
+        <v>3.5</v>
       </c>
     </row>
     <row r="239" spans="1:4">
@@ -1926,15 +1926,15 @@
     <row r="241" spans="1:4">
       <c r="A241">
         <f>A61*D241*A201*A53*C10</f>
-        <v>7315350.0330990553</v>
+        <v>26848514.793580521</v>
       </c>
       <c r="B241">
         <f>A241/10000000</f>
-        <v>0.73153500330990551</v>
+        <v>2.684851479358052</v>
       </c>
       <c r="D241">
-        <f>2*B30+A77/C6</f>
-        <v>0.95363655355597343</v>
+        <f>2*B30+C18</f>
+        <v>3.5</v>
       </c>
     </row>
     <row r="243" spans="1:4">
@@ -1951,15 +1951,15 @@
     <row r="245" spans="1:4">
       <c r="A245">
         <f>A65*D245*40*A205</f>
-        <v>19387295.153210171</v>
+        <v>14383132.925132422</v>
       </c>
       <c r="B245">
         <f>A245/10000000</f>
-        <v>1.9387295153210171</v>
+        <v>1.4383132925132422</v>
       </c>
       <c r="D245">
-        <f>2*B30+A81/D6</f>
-        <v>1.3479187916934081</v>
+        <f>2*B30+D18</f>
+        <v>1</v>
       </c>
     </row>
     <row r="247" spans="1:4">
@@ -1973,11 +1973,11 @@
     <row r="249" spans="1:4">
       <c r="A249">
         <f>A245+A241+A237</f>
-        <v>80376082.442400098</v>
+        <v>238221821.48651391</v>
       </c>
       <c r="B249">
         <f>A249/10000000</f>
-        <v>8.0376082442400101</v>
+        <v>23.82218214865139</v>
       </c>
     </row>
     <row r="251" spans="1:4">
@@ -1988,7 +1988,7 @@
     <row r="253" spans="1:4">
       <c r="A253">
         <f>A249/B2/1000</f>
-        <v>80.376082442400104</v>
+        <v>238.2218214865139</v>
       </c>
     </row>
     <row r="255" spans="1:4">
@@ -1999,7 +1999,7 @@
     <row r="257" spans="1:1">
       <c r="A257">
         <f>A233+B35*(B24 +A253)/(8769*B22)</f>
-        <v>8.6365081187425072E-2</v>
+        <v>8.7452328214037478E-2</v>
       </c>
     </row>
     <row r="259" spans="1:1">
@@ -2010,7 +2010,7 @@
     <row r="261" spans="1:1">
       <c r="A261">
         <f>((0.0707-A233)*8760*B22-B35*A253)/B35</f>
-        <v>937.48123442992403</v>
+        <v>863.72249095460165</v>
       </c>
     </row>
   </sheetData>

</xml_diff>